<commit_message>
Avoiding using fixed row indexes in LandPracticeSystemsBuilder.
</commit_message>
<xml_diff>
--- a/test/land_practice_systems.xlsx
+++ b/test/land_practice_systems.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="184" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="526"/>
   </bookViews>
   <sheets>
-    <sheet name="horticulture" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="sugarcane" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="grains" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="horticulture" sheetId="1" r:id="rId1"/>
+    <sheet name="sugarcane" sheetId="2" r:id="rId2"/>
+    <sheet name="grains" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -56,9 +59,6 @@
     <t>cape york</t>
   </si>
   <si>
-    <t>wet toprics</t>
-  </si>
-  <si>
     <t>burdekin</t>
   </si>
   <si>
@@ -70,43 +70,27 @@
   <si>
     <t>burnett mary</t>
   </si>
+  <si>
+    <t>wet tropics</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00%" numFmtId="165"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,7 +102,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -126,79 +110,321 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E15" activeCellId="1" pane="topLeft" sqref="J5:M5 E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.82352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.6313725490196"/>
+    <col min="1" max="1" width="19.5703125"/>
+    <col min="2" max="8" width="11.5703125"/>
+    <col min="9" max="9" width="9.85546875"/>
+    <col min="10" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -214,7 +440,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -252,90 +478,90 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D4" s="5" t="n">
+      <c r="B4" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D4" s="5">
         <v>0.37</v>
       </c>
-      <c r="E4" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G4" s="5" t="n">
+      <c r="E4" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G4" s="5">
         <v>0.5</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="5">
         <v>0.16</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="5">
         <v>0.06</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="5">
         <v>0.3</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="5">
         <v>0.4</v>
       </c>
-      <c r="L4" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M4" s="5" t="n">
+      <c r="L4" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M4" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D5" s="5" t="n">
+      <c r="B5" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D5" s="5">
         <v>0.32</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G5" s="5" t="n">
+      <c r="E5" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G5" s="5">
         <v>0.53</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="5">
         <v>0.2</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="5">
         <v>0.04</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="5">
         <v>0.27</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="5">
         <v>0.35</v>
       </c>
-      <c r="L5" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M5" s="5" t="n">
+      <c r="L5" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M5" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -351,7 +577,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -389,91 +615,91 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="5">
         <v>0.25</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="5">
         <v>0.03</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="5">
         <v>0.44</v>
       </c>
-      <c r="E9" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="F9" s="5" t="n">
+      <c r="E9" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F9" s="5">
         <v>0.09</v>
       </c>
-      <c r="G9" s="5" t="n">
-        <v>0.56</v>
-      </c>
-      <c r="H9" s="5" t="n">
+      <c r="G9" s="5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H9" s="5">
         <v>0.16</v>
       </c>
-      <c r="I9" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="J9" s="5" t="n">
+      <c r="I9" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="J9" s="5">
         <v>0.3</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="5">
         <v>0.11</v>
       </c>
-      <c r="L9" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M9" s="5" t="n">
+      <c r="L9" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M9" s="5">
         <v>0.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D10" s="5" t="n">
+      <c r="B10" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D10" s="5">
         <v>0.32</v>
       </c>
-      <c r="E10" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F10" s="5" t="n">
+      <c r="E10" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F10" s="5">
         <v>0.25</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="5">
         <v>0.25</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="5">
         <v>0.25</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="5">
         <v>0.25</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" s="5">
         <v>0.22</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="5">
         <v>0.01</v>
       </c>
-      <c r="L10" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M10" s="5" t="n">
+      <c r="L10" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M10" s="5">
         <v>0.48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
-        <v>12</v>
+    <row r="12" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
@@ -488,7 +714,7 @@
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -526,91 +752,91 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="5">
         <v>0.12</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="5">
         <v>0.12</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="5">
         <v>0.12</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="5">
         <v>0.64</v>
       </c>
-      <c r="F14" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G14" s="5" t="n">
+      <c r="F14" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G14" s="5">
         <v>0.5</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="5">
         <v>0.16</v>
       </c>
-      <c r="I14" s="5" t="n">
+      <c r="I14" s="5">
         <v>0.06</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" s="5">
         <v>0.3</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="5">
         <v>0.4</v>
       </c>
-      <c r="L14" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M14" s="5" t="n">
+      <c r="L14" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M14" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="5">
         <v>0.02</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="5">
         <v>0.02</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="5">
         <v>0.02</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="5">
         <v>0.94</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="5">
         <v>0.33</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="5">
         <v>0.33</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="5">
         <v>0.33</v>
       </c>
-      <c r="I15" s="5" t="n">
+      <c r="I15" s="5">
         <v>0.01</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" s="5">
         <v>0.2</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="5">
         <v>0.2</v>
       </c>
-      <c r="L15" s="5" t="n">
+      <c r="L15" s="5">
         <v>0.2</v>
       </c>
-      <c r="M15" s="5" t="n">
+      <c r="M15" s="5">
         <v>0.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
-        <v>13</v>
+    <row r="17" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -625,7 +851,7 @@
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -663,91 +889,91 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row r="19" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D19" s="5" t="n">
+      <c r="B19" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D19" s="5">
         <v>0.37</v>
       </c>
-      <c r="E19" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G19" s="5" t="n">
+      <c r="E19" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G19" s="5">
         <v>0.5</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="5">
         <v>0.16</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="I19" s="5">
         <v>0.06</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" s="5">
         <v>0.3</v>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="K19" s="5">
         <v>0.4</v>
       </c>
-      <c r="L19" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M19" s="5" t="n">
+      <c r="L19" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M19" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row r="20" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C20" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D20" s="5" t="n">
+      <c r="B20" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D20" s="5">
         <v>0.32</v>
       </c>
-      <c r="E20" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G20" s="5" t="n">
+      <c r="E20" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G20" s="5">
         <v>0.53</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="H20" s="5">
         <v>0.2</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="I20" s="5">
         <v>0.04</v>
       </c>
-      <c r="J20" s="5" t="n">
+      <c r="J20" s="5">
         <v>0.27</v>
       </c>
-      <c r="K20" s="5" t="n">
+      <c r="K20" s="5">
         <v>0.35</v>
       </c>
-      <c r="L20" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M20" s="5" t="n">
+      <c r="L20" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M20" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
-      <c r="A22" s="0" t="s">
-        <v>14</v>
+    <row r="22" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>2</v>
@@ -762,7 +988,7 @@
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row r="23" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
@@ -800,91 +1026,91 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row r="24" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D24" s="5" t="n">
+      <c r="B24" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D24" s="5">
         <v>0.37</v>
       </c>
-      <c r="E24" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F24" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G24" s="5" t="n">
+      <c r="E24" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G24" s="5">
         <v>0.5</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" s="5">
         <v>0.16</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="I24" s="5">
         <v>0.06</v>
       </c>
-      <c r="J24" s="5" t="n">
+      <c r="J24" s="5">
         <v>0.3</v>
       </c>
-      <c r="K24" s="5" t="n">
+      <c r="K24" s="5">
         <v>0.4</v>
       </c>
-      <c r="L24" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M24" s="5" t="n">
+      <c r="L24" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M24" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row r="25" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D25" s="5" t="n">
+      <c r="B25" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D25" s="5">
         <v>0.32</v>
       </c>
-      <c r="E25" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F25" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G25" s="5" t="n">
+      <c r="E25" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G25" s="5">
         <v>0.53</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="H25" s="5">
         <v>0.2</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" s="5">
         <v>0.04</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="J25" s="5">
         <v>0.27</v>
       </c>
-      <c r="K25" s="5" t="n">
+      <c r="K25" s="5">
         <v>0.35</v>
       </c>
-      <c r="L25" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M25" s="5" t="n">
+      <c r="L25" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M25" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="s">
-        <v>15</v>
+    <row r="27" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>2</v>
@@ -899,7 +1125,7 @@
       </c>
       <c r="L27" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row r="28" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
@@ -937,91 +1163,91 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row r="29" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D29" s="5" t="n">
+      <c r="B29" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D29" s="5">
         <v>0.37</v>
       </c>
-      <c r="E29" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F29" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G29" s="5" t="n">
+      <c r="E29" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G29" s="5">
         <v>0.5</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" s="5">
         <v>0.16</v>
       </c>
-      <c r="I29" s="5" t="n">
+      <c r="I29" s="5">
         <v>0.06</v>
       </c>
-      <c r="J29" s="5" t="n">
+      <c r="J29" s="5">
         <v>0.3</v>
       </c>
-      <c r="K29" s="5" t="n">
+      <c r="K29" s="5">
         <v>0.4</v>
       </c>
-      <c r="L29" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M29" s="5" t="n">
+      <c r="L29" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M29" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row r="30" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D30" s="5" t="n">
+      <c r="B30" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D30" s="5">
         <v>0.32</v>
       </c>
-      <c r="E30" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F30" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G30" s="5" t="n">
+      <c r="E30" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G30" s="5">
         <v>0.53</v>
       </c>
-      <c r="H30" s="5" t="n">
+      <c r="H30" s="5">
         <v>0.2</v>
       </c>
-      <c r="I30" s="5" t="n">
+      <c r="I30" s="5">
         <v>0.04</v>
       </c>
-      <c r="J30" s="5" t="n">
+      <c r="J30" s="5">
         <v>0.27</v>
       </c>
-      <c r="K30" s="5" t="n">
+      <c r="K30" s="5">
         <v>0.35</v>
       </c>
-      <c r="L30" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M30" s="5" t="n">
+      <c r="L30" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M30" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="0" t="s">
-        <v>16</v>
+    <row r="32" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>2</v>
@@ -1036,7 +1262,7 @@
       </c>
       <c r="L32" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row r="33" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
@@ -1074,93 +1300,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row r="34" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D34" s="5" t="n">
+      <c r="B34" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D34" s="5">
         <v>0.37</v>
       </c>
-      <c r="E34" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G34" s="5" t="n">
+      <c r="E34" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G34" s="5">
         <v>0.5</v>
       </c>
-      <c r="H34" s="5" t="n">
+      <c r="H34" s="5">
         <v>0.16</v>
       </c>
-      <c r="I34" s="5" t="n">
+      <c r="I34" s="5">
         <v>0.06</v>
       </c>
-      <c r="J34" s="5" t="n">
+      <c r="J34" s="5">
         <v>0.3</v>
       </c>
-      <c r="K34" s="5" t="n">
+      <c r="K34" s="5">
         <v>0.4</v>
       </c>
-      <c r="L34" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M34" s="5" t="n">
+      <c r="L34" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M34" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row r="35" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C35" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D35" s="5" t="n">
+      <c r="B35" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D35" s="5">
         <v>0.32</v>
       </c>
-      <c r="E35" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F35" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G35" s="5" t="n">
+      <c r="E35" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G35" s="5">
         <v>0.53</v>
       </c>
-      <c r="H35" s="5" t="n">
+      <c r="H35" s="5">
         <v>0.2</v>
       </c>
-      <c r="I35" s="5" t="n">
+      <c r="I35" s="5">
         <v>0.04</v>
       </c>
-      <c r="J35" s="5" t="n">
+      <c r="J35" s="5">
         <v>0.27</v>
       </c>
-      <c r="K35" s="5" t="n">
+      <c r="K35" s="5">
         <v>0.35</v>
       </c>
-      <c r="L35" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M35" s="5" t="n">
+      <c r="L35" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M35" s="5">
         <v>0.09</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1168,23 +1393,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M35"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="J5:M5 A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6313725490196"/>
+    <col min="1" max="1" width="17.7109375"/>
+    <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1200,7 +1423,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1238,91 +1461,91 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D4" s="5" t="n">
+      <c r="B4" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D4" s="5">
         <v>0.37</v>
       </c>
-      <c r="E4" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G4" s="5" t="n">
+      <c r="E4" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G4" s="5">
         <v>0.5</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="5">
         <v>0.16</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="5">
         <v>0.06</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="5">
         <v>0.3</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="5">
         <v>0.4</v>
       </c>
-      <c r="L4" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M4" s="5" t="n">
+      <c r="L4" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M4" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D5" s="5" t="n">
+      <c r="B5" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D5" s="5">
         <v>0.32</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G5" s="5" t="n">
+      <c r="E5" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G5" s="5">
         <v>0.53</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="5">
         <v>0.2</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="5">
         <v>0.04</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="5">
         <v>0.27</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="5">
         <v>0.35</v>
       </c>
-      <c r="L5" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M5" s="5" t="n">
+      <c r="L5" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M5" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="6" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1338,7 +1561,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1376,92 +1599,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D9" s="5" t="n">
+      <c r="B9" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D9" s="5">
         <v>0.37</v>
       </c>
-      <c r="E9" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G9" s="5" t="n">
+      <c r="E9" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G9" s="5">
         <v>0.5</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="5">
         <v>0.16</v>
       </c>
-      <c r="I9" s="5" t="n">
+      <c r="I9" s="5">
         <v>0.06</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="5">
         <v>0.3</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="5">
         <v>0.4</v>
       </c>
-      <c r="L9" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M9" s="5" t="n">
+      <c r="L9" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M9" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D10" s="5" t="n">
+      <c r="B10" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D10" s="5">
         <v>0.32</v>
       </c>
-      <c r="E10" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G10" s="5" t="n">
+      <c r="E10" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G10" s="5">
         <v>0.53</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="5">
         <v>0.2</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="5">
         <v>0.04</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" s="5">
         <v>0.27</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="5">
         <v>0.35</v>
       </c>
-      <c r="L10" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M10" s="5" t="n">
+      <c r="L10" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M10" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
-        <v>12</v>
+    <row r="11" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
@@ -1476,7 +1699,7 @@
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1514,92 +1737,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D14" s="5" t="n">
+      <c r="B14" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D14" s="5">
         <v>0.37</v>
       </c>
-      <c r="E14" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G14" s="5" t="n">
+      <c r="E14" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G14" s="5">
         <v>0.5</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="5">
         <v>0.16</v>
       </c>
-      <c r="I14" s="5" t="n">
+      <c r="I14" s="5">
         <v>0.06</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" s="5">
         <v>0.3</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="5">
         <v>0.4</v>
       </c>
-      <c r="L14" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M14" s="5" t="n">
+      <c r="L14" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M14" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D15" s="5" t="n">
+      <c r="B15" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D15" s="5">
         <v>0.32</v>
       </c>
-      <c r="E15" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G15" s="5" t="n">
+      <c r="E15" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G15" s="5">
         <v>0.53</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="5">
         <v>0.2</v>
       </c>
-      <c r="I15" s="5" t="n">
+      <c r="I15" s="5">
         <v>0.04</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" s="5">
         <v>0.27</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="5">
         <v>0.35</v>
       </c>
-      <c r="L15" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M15" s="5" t="n">
+      <c r="L15" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M15" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
-        <v>13</v>
+    <row r="16" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -1614,7 +1837,7 @@
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1652,92 +1875,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row r="19" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D19" s="5" t="n">
+      <c r="B19" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D19" s="5">
         <v>0.37</v>
       </c>
-      <c r="E19" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G19" s="5" t="n">
+      <c r="E19" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G19" s="5">
         <v>0.5</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="5">
         <v>0.16</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="I19" s="5">
         <v>0.06</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" s="5">
         <v>0.3</v>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="K19" s="5">
         <v>0.4</v>
       </c>
-      <c r="L19" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M19" s="5" t="n">
+      <c r="L19" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M19" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row r="20" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C20" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D20" s="5" t="n">
+      <c r="B20" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D20" s="5">
         <v>0.32</v>
       </c>
-      <c r="E20" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G20" s="5" t="n">
+      <c r="E20" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G20" s="5">
         <v>0.53</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="H20" s="5">
         <v>0.2</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="I20" s="5">
         <v>0.04</v>
       </c>
-      <c r="J20" s="5" t="n">
+      <c r="J20" s="5">
         <v>0.27</v>
       </c>
-      <c r="K20" s="5" t="n">
+      <c r="K20" s="5">
         <v>0.35</v>
       </c>
-      <c r="L20" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M20" s="5" t="n">
+      <c r="L20" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M20" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
-      <c r="A22" s="0" t="s">
-        <v>14</v>
+    <row r="21" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>2</v>
@@ -1752,7 +1975,7 @@
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row r="23" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
@@ -1790,92 +2013,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row r="24" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D24" s="5" t="n">
+      <c r="B24" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D24" s="5">
         <v>0.37</v>
       </c>
-      <c r="E24" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F24" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G24" s="5" t="n">
+      <c r="E24" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G24" s="5">
         <v>0.5</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" s="5">
         <v>0.16</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="I24" s="5">
         <v>0.06</v>
       </c>
-      <c r="J24" s="5" t="n">
+      <c r="J24" s="5">
         <v>0.3</v>
       </c>
-      <c r="K24" s="5" t="n">
+      <c r="K24" s="5">
         <v>0.4</v>
       </c>
-      <c r="L24" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M24" s="5" t="n">
+      <c r="L24" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M24" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row r="25" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D25" s="5" t="n">
+      <c r="B25" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D25" s="5">
         <v>0.32</v>
       </c>
-      <c r="E25" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F25" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G25" s="5" t="n">
+      <c r="E25" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G25" s="5">
         <v>0.53</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="H25" s="5">
         <v>0.2</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" s="5">
         <v>0.04</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="J25" s="5">
         <v>0.27</v>
       </c>
-      <c r="K25" s="5" t="n">
+      <c r="K25" s="5">
         <v>0.35</v>
       </c>
-      <c r="L25" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M25" s="5" t="n">
+      <c r="L25" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M25" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="s">
-        <v>15</v>
+    <row r="26" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>2</v>
@@ -1890,7 +2113,7 @@
       </c>
       <c r="L27" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row r="28" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
@@ -1928,92 +2151,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row r="29" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D29" s="5" t="n">
+      <c r="B29" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D29" s="5">
         <v>0.37</v>
       </c>
-      <c r="E29" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F29" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G29" s="5" t="n">
+      <c r="E29" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G29" s="5">
         <v>0.5</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" s="5">
         <v>0.16</v>
       </c>
-      <c r="I29" s="5" t="n">
+      <c r="I29" s="5">
         <v>0.06</v>
       </c>
-      <c r="J29" s="5" t="n">
+      <c r="J29" s="5">
         <v>0.3</v>
       </c>
-      <c r="K29" s="5" t="n">
+      <c r="K29" s="5">
         <v>0.4</v>
       </c>
-      <c r="L29" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M29" s="5" t="n">
+      <c r="L29" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M29" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row r="30" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D30" s="5" t="n">
+      <c r="B30" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D30" s="5">
         <v>0.32</v>
       </c>
-      <c r="E30" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F30" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G30" s="5" t="n">
+      <c r="E30" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G30" s="5">
         <v>0.53</v>
       </c>
-      <c r="H30" s="5" t="n">
+      <c r="H30" s="5">
         <v>0.2</v>
       </c>
-      <c r="I30" s="5" t="n">
+      <c r="I30" s="5">
         <v>0.04</v>
       </c>
-      <c r="J30" s="5" t="n">
+      <c r="J30" s="5">
         <v>0.27</v>
       </c>
-      <c r="K30" s="5" t="n">
+      <c r="K30" s="5">
         <v>0.35</v>
       </c>
-      <c r="L30" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M30" s="5" t="n">
+      <c r="L30" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M30" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="0" t="s">
-        <v>16</v>
+    <row r="31" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>2</v>
@@ -2028,7 +2251,7 @@
       </c>
       <c r="L32" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row r="33" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
@@ -2066,93 +2289,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row r="34" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D34" s="5" t="n">
+      <c r="B34" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D34" s="5">
         <v>0.37</v>
       </c>
-      <c r="E34" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G34" s="5" t="n">
+      <c r="E34" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G34" s="5">
         <v>0.5</v>
       </c>
-      <c r="H34" s="5" t="n">
+      <c r="H34" s="5">
         <v>0.16</v>
       </c>
-      <c r="I34" s="5" t="n">
+      <c r="I34" s="5">
         <v>0.06</v>
       </c>
-      <c r="J34" s="5" t="n">
+      <c r="J34" s="5">
         <v>0.3</v>
       </c>
-      <c r="K34" s="5" t="n">
+      <c r="K34" s="5">
         <v>0.4</v>
       </c>
-      <c r="L34" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M34" s="5" t="n">
+      <c r="L34" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M34" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row r="35" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C35" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D35" s="5" t="n">
+      <c r="B35" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D35" s="5">
         <v>0.32</v>
       </c>
-      <c r="E35" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F35" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G35" s="5" t="n">
+      <c r="E35" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G35" s="5">
         <v>0.53</v>
       </c>
-      <c r="H35" s="5" t="n">
+      <c r="H35" s="5">
         <v>0.2</v>
       </c>
-      <c r="I35" s="5" t="n">
+      <c r="I35" s="5">
         <v>0.04</v>
       </c>
-      <c r="J35" s="5" t="n">
+      <c r="J35" s="5">
         <v>0.27</v>
       </c>
-      <c r="K35" s="5" t="n">
+      <c r="K35" s="5">
         <v>0.35</v>
       </c>
-      <c r="L35" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M35" s="5" t="n">
+      <c r="L35" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M35" s="5">
         <v>0.09</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2160,23 +2382,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M35"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J5" activeCellId="0" pane="topLeft" sqref="J5:M5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6313725490196"/>
+    <col min="1" max="1" width="17.7109375"/>
+    <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2192,7 +2412,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2230,91 +2450,91 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="5">
         <v>0.01</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="5">
         <v>0.01</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="5">
         <v>0.01</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="5">
         <v>0.97</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="5">
         <v>0.25</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="5">
         <v>0.25</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="5">
         <v>0.25</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="5">
         <v>0.25</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="5">
         <v>0.33</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="5">
         <v>0.33</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="5">
         <v>0.33</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="5">
         <v>0.01</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="5">
         <v>0.97</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="5">
         <v>0.01</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="5">
         <v>0.01</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="5">
         <v>0.01</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="5">
         <v>0.25</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="5">
         <v>0.25</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="5">
         <v>0.25</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="5">
         <v>0.25</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="5">
         <v>0.01</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="5">
         <v>0.33</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="5">
         <v>0.33</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="5">
         <v>0.33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="6" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2330,7 +2550,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2368,92 +2588,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D9" s="5" t="n">
+      <c r="B9" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D9" s="5">
         <v>0.37</v>
       </c>
-      <c r="E9" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G9" s="5" t="n">
+      <c r="E9" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G9" s="5">
         <v>0.5</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="5">
         <v>0.16</v>
       </c>
-      <c r="I9" s="5" t="n">
+      <c r="I9" s="5">
         <v>0.06</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="5">
         <v>0.3</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="5">
         <v>0.4</v>
       </c>
-      <c r="L9" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M9" s="5" t="n">
+      <c r="L9" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M9" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D10" s="5" t="n">
+      <c r="B10" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D10" s="5">
         <v>0.32</v>
       </c>
-      <c r="E10" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G10" s="5" t="n">
+      <c r="E10" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G10" s="5">
         <v>0.53</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="5">
         <v>0.2</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="5">
         <v>0.04</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" s="5">
         <v>0.27</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="5">
         <v>0.35</v>
       </c>
-      <c r="L10" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M10" s="5" t="n">
+      <c r="L10" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M10" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
-        <v>12</v>
+    <row r="11" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
@@ -2468,7 +2688,7 @@
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -2506,92 +2726,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D14" s="5" t="n">
+      <c r="B14" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D14" s="5">
         <v>0.37</v>
       </c>
-      <c r="E14" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G14" s="5" t="n">
+      <c r="E14" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G14" s="5">
         <v>0.5</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="5">
         <v>0.16</v>
       </c>
-      <c r="I14" s="5" t="n">
+      <c r="I14" s="5">
         <v>0.06</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" s="5">
         <v>0.3</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="5">
         <v>0.4</v>
       </c>
-      <c r="L14" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M14" s="5" t="n">
+      <c r="L14" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M14" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D15" s="5" t="n">
+      <c r="B15" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D15" s="5">
         <v>0.32</v>
       </c>
-      <c r="E15" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G15" s="5" t="n">
+      <c r="E15" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G15" s="5">
         <v>0.53</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="5">
         <v>0.2</v>
       </c>
-      <c r="I15" s="5" t="n">
+      <c r="I15" s="5">
         <v>0.04</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" s="5">
         <v>0.27</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="5">
         <v>0.35</v>
       </c>
-      <c r="L15" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M15" s="5" t="n">
+      <c r="L15" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M15" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
-        <v>13</v>
+    <row r="16" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -2606,7 +2826,7 @@
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -2644,92 +2864,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row r="19" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D19" s="5" t="n">
+      <c r="B19" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D19" s="5">
         <v>0.37</v>
       </c>
-      <c r="E19" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G19" s="5" t="n">
+      <c r="E19" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G19" s="5">
         <v>0.5</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="5">
         <v>0.16</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="I19" s="5">
         <v>0.06</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" s="5">
         <v>0.3</v>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="K19" s="5">
         <v>0.4</v>
       </c>
-      <c r="L19" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M19" s="5" t="n">
+      <c r="L19" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M19" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row r="20" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C20" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D20" s="5" t="n">
+      <c r="B20" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D20" s="5">
         <v>0.32</v>
       </c>
-      <c r="E20" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G20" s="5" t="n">
+      <c r="E20" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G20" s="5">
         <v>0.53</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="H20" s="5">
         <v>0.2</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="I20" s="5">
         <v>0.04</v>
       </c>
-      <c r="J20" s="5" t="n">
+      <c r="J20" s="5">
         <v>0.27</v>
       </c>
-      <c r="K20" s="5" t="n">
+      <c r="K20" s="5">
         <v>0.35</v>
       </c>
-      <c r="L20" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M20" s="5" t="n">
+      <c r="L20" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M20" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
-      <c r="A22" s="0" t="s">
-        <v>14</v>
+    <row r="21" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>2</v>
@@ -2744,7 +2964,7 @@
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row r="23" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
@@ -2782,92 +3002,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row r="24" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D24" s="5" t="n">
+      <c r="B24" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D24" s="5">
         <v>0.37</v>
       </c>
-      <c r="E24" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F24" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G24" s="5" t="n">
+      <c r="E24" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G24" s="5">
         <v>0.5</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" s="5">
         <v>0.16</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="I24" s="5">
         <v>0.06</v>
       </c>
-      <c r="J24" s="5" t="n">
+      <c r="J24" s="5">
         <v>0.3</v>
       </c>
-      <c r="K24" s="5" t="n">
+      <c r="K24" s="5">
         <v>0.4</v>
       </c>
-      <c r="L24" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M24" s="5" t="n">
+      <c r="L24" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M24" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row r="25" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D25" s="5" t="n">
+      <c r="B25" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D25" s="5">
         <v>0.32</v>
       </c>
-      <c r="E25" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F25" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G25" s="5" t="n">
+      <c r="E25" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G25" s="5">
         <v>0.53</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="H25" s="5">
         <v>0.2</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" s="5">
         <v>0.04</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="J25" s="5">
         <v>0.27</v>
       </c>
-      <c r="K25" s="5" t="n">
+      <c r="K25" s="5">
         <v>0.35</v>
       </c>
-      <c r="L25" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M25" s="5" t="n">
+      <c r="L25" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M25" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="s">
-        <v>15</v>
+    <row r="26" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>2</v>
@@ -2882,7 +3102,7 @@
       </c>
       <c r="L27" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row r="28" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
@@ -2920,92 +3140,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row r="29" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D29" s="5" t="n">
+      <c r="B29" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D29" s="5">
         <v>0.37</v>
       </c>
-      <c r="E29" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F29" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G29" s="5" t="n">
+      <c r="E29" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G29" s="5">
         <v>0.5</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" s="5">
         <v>0.16</v>
       </c>
-      <c r="I29" s="5" t="n">
+      <c r="I29" s="5">
         <v>0.06</v>
       </c>
-      <c r="J29" s="5" t="n">
+      <c r="J29" s="5">
         <v>0.3</v>
       </c>
-      <c r="K29" s="5" t="n">
+      <c r="K29" s="5">
         <v>0.4</v>
       </c>
-      <c r="L29" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M29" s="5" t="n">
+      <c r="L29" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M29" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row r="30" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D30" s="5" t="n">
+      <c r="B30" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D30" s="5">
         <v>0.32</v>
       </c>
-      <c r="E30" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F30" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G30" s="5" t="n">
+      <c r="E30" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G30" s="5">
         <v>0.53</v>
       </c>
-      <c r="H30" s="5" t="n">
+      <c r="H30" s="5">
         <v>0.2</v>
       </c>
-      <c r="I30" s="5" t="n">
+      <c r="I30" s="5">
         <v>0.04</v>
       </c>
-      <c r="J30" s="5" t="n">
+      <c r="J30" s="5">
         <v>0.27</v>
       </c>
-      <c r="K30" s="5" t="n">
+      <c r="K30" s="5">
         <v>0.35</v>
       </c>
-      <c r="L30" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M30" s="5" t="n">
+      <c r="L30" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M30" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="0" t="s">
-        <v>16</v>
+    <row r="31" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>2</v>
@@ -3020,7 +3240,7 @@
       </c>
       <c r="L32" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row r="33" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
@@ -3058,118 +3278,92 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row r="34" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D34" s="5" t="n">
+      <c r="B34" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="D34" s="5">
         <v>0.37</v>
       </c>
-      <c r="E34" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="G34" s="5" t="n">
+      <c r="E34" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G34" s="5">
         <v>0.5</v>
       </c>
-      <c r="H34" s="5" t="n">
+      <c r="H34" s="5">
         <v>0.16</v>
       </c>
-      <c r="I34" s="5" t="n">
+      <c r="I34" s="5">
         <v>0.06</v>
       </c>
-      <c r="J34" s="5" t="n">
+      <c r="J34" s="5">
         <v>0.3</v>
       </c>
-      <c r="K34" s="5" t="n">
+      <c r="K34" s="5">
         <v>0.4</v>
       </c>
-      <c r="L34" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="M34" s="5" t="n">
+      <c r="L34" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="M34" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row r="35" spans="1:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="5" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C35" s="5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D35" s="5" t="n">
+      <c r="B35" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D35" s="5">
         <v>0.32</v>
       </c>
-      <c r="E35" s="5" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F35" s="5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="G35" s="5" t="n">
+      <c r="E35" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="G35" s="5">
         <v>0.53</v>
       </c>
-      <c r="H35" s="5" t="n">
+      <c r="H35" s="5">
         <v>0.2</v>
       </c>
-      <c r="I35" s="5" t="n">
+      <c r="I35" s="5">
         <v>0.04</v>
       </c>
-      <c r="J35" s="5" t="n">
+      <c r="J35" s="5">
         <v>0.27</v>
       </c>
-      <c r="K35" s="5" t="n">
+      <c r="K35" s="5">
         <v>0.35</v>
       </c>
-      <c r="L35" s="5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M35" s="5" t="n">
+      <c r="L35" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M35" s="5">
         <v>0.09</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="J5:M5 A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>